<commit_message>
SSDM-12286 Added export support for data sets.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE429D74-1D57-C343-811F-CA27B03C9EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B23500-932E-8841-9BCD-FB058A8664A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="17120" windowHeight="13100" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="27320" windowHeight="17500" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Code</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -59,15 +56,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>This is Test 1</t>
-  </si>
-  <si>
-    <t>This is Test 3</t>
-  </si>
-  <si>
-    <t>This is Test 2</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
@@ -77,18 +65,12 @@
     <t>Test 3</t>
   </si>
   <si>
-    <t>/TEST/TEST/TEST_1</t>
-  </si>
-  <si>
     <t>TEST_1</t>
   </si>
   <si>
     <t>/TEST/TEST_1</t>
   </si>
   <si>
-    <t>/TEST/TEST/TEST_2</t>
-  </si>
-  <si>
     <t>TEST_2</t>
   </si>
   <si>
@@ -98,9 +80,6 @@
     <t>/TEST/TEST_2</t>
   </si>
   <si>
-    <t>/TEST/TEST/TEST_3</t>
-  </si>
-  <si>
     <t>TEST_3</t>
   </si>
   <si>
@@ -108,6 +87,20 @@
   </si>
   <si>
     <t>Experiment</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>file1.bin</t>
+  </si>
+  <si>
+    <t>file2.bin</t>
+  </si>
+  <si>
+    <t>This is
+multiline
+text.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -178,6 +171,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC7960-BC38-5143-9487-091D72DFAD39}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,128 +505,113 @@
     <col min="9" max="9" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>